<commit_message>
First login for MENTEES
</commit_message>
<xml_diff>
--- a/webapp/resources/errorHandling.xlsx
+++ b/webapp/resources/errorHandling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\wamp64\www\adhere\webapp\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B745E88B-A74A-4AD6-81A8-E920E9540A7F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EBBFD9-4A60-434E-AB68-81D9EE481DAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" xr2:uid="{8EC083B6-2DF0-4B4C-8317-1543DA186256}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490" xr2:uid="{8EC083B6-2DF0-4B4C-8317-1543DA186256}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -493,30 +493,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F88DFB-1C99-4257-A837-997F6E433A26}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="43.77734375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="43.7109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -527,7 +527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>35</v>
       </c>
@@ -538,7 +538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>51</v>
       </c>
@@ -549,19 +549,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -572,7 +572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>93</v>
       </c>
@@ -583,7 +583,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>39</v>
       </c>
@@ -594,7 +594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>61</v>
       </c>
@@ -605,19 +605,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -628,7 +628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>18</v>
       </c>
@@ -639,19 +639,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -662,7 +662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -673,19 +673,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
@@ -696,7 +696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>10</v>
       </c>
@@ -707,7 +707,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>20</v>
       </c>
@@ -718,19 +718,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
@@ -741,7 +741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>30</v>
       </c>
@@ -752,19 +752,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>1</v>
       </c>
@@ -775,7 +775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>10</v>
       </c>
@@ -786,7 +786,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>21</v>
       </c>
@@ -797,19 +797,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>1</v>
       </c>
@@ -820,7 +820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>17</v>
       </c>
@@ -831,19 +831,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>1</v>
       </c>
@@ -854,7 +854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>22</v>
       </c>
@@ -865,19 +865,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>1</v>
       </c>
@@ -888,7 +888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>27</v>
       </c>
@@ -899,19 +899,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>1</v>
       </c>
@@ -922,7 +922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>41</v>
       </c>
@@ -933,7 +933,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>75</v>
       </c>
@@ -944,19 +944,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>1</v>
       </c>
@@ -967,7 +967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>33</v>
       </c>
@@ -980,11 +980,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="A12:C13"/>
-    <mergeCell ref="A17:C18"/>
-    <mergeCell ref="A21:C22"/>
     <mergeCell ref="A47:C48"/>
     <mergeCell ref="A52:C53"/>
     <mergeCell ref="A26:C27"/>
@@ -992,6 +987,11 @@
     <mergeCell ref="A35:C36"/>
     <mergeCell ref="A39:C40"/>
     <mergeCell ref="A43:C44"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="A12:C13"/>
+    <mergeCell ref="A17:C18"/>
+    <mergeCell ref="A21:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>